<commit_message>
added the tests cases
</commit_message>
<xml_diff>
--- a/static/assets/resit_exam_details_template.xlsx
+++ b/static/assets/resit_exam_details_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djeid\OneDrive\cs projects\se302_resit_backend\static\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F71830D-CCBE-4FAD-8C8F-EE4040AE72C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A19C0A52-5BC2-483D-BC29-0168BD182479}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2196" yWindow="2196" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>num_questions</t>
   </si>
@@ -35,18 +35,6 @@
   </si>
   <si>
     <t>additional_notes</t>
-  </si>
-  <si>
-    <t>multtiple choice</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>ayhan at 9 am</t>
-  </si>
-  <si>
-    <t>bring food with u</t>
   </si>
 </sst>
 </file>
@@ -414,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -446,23 +434,6 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>20</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>